<commit_message>
added new presentation and added new workflow
</commit_message>
<xml_diff>
--- a/logs/user_performance.xlsx
+++ b/logs/user_performance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\computer_vision_pptx_controller\logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CB53B4B-6C99-4571-8EC4-5FEA30E4F009}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D72A49C-7581-4806-A82A-451895BCDA3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -425,9 +425,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="A3:G3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
added excel file regarding user performance
</commit_message>
<xml_diff>
--- a/logs/user_performance.xlsx
+++ b/logs/user_performance.xlsx
@@ -1,71 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\computer_vision_pptx_controller\logs\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D72A49C-7581-4806-A82A-451895BCDA3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="List1" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="List1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
-  <si>
-    <t>Specific</t>
-  </si>
-  <si>
-    <t>Counting</t>
-  </si>
-  <si>
-    <t>User</t>
-  </si>
-  <si>
-    <t>Flow 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Error number 1</t>
-  </si>
-  <si>
-    <t>Flow 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Error number 2</t>
-  </si>
-  <si>
-    <t>Flow 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Error number 3</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
+      <name val="Aptos Narrow"/>
+      <charset val="238"/>
+      <family val="2"/>
+      <color theme="1"/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <charset val="238"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -84,25 +47,84 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalno" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -422,89 +444,502 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="36.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col width="36.85546875" bestFit="1" customWidth="1" style="2" min="1" max="1"/>
+    <col width="6.5703125" bestFit="1" customWidth="1" style="2" min="2" max="2"/>
+    <col width="14.5703125" bestFit="1" customWidth="1" style="2" min="3" max="3"/>
+    <col width="6.5703125" bestFit="1" customWidth="1" style="2" min="4" max="4"/>
+    <col width="14.5703125" bestFit="1" customWidth="1" style="2" min="5" max="5"/>
+    <col width="6.5703125" bestFit="1" customWidth="1" style="2" min="6" max="6"/>
+    <col width="14.5703125" bestFit="1" customWidth="1" style="2" min="7" max="7"/>
+    <col width="6.5703125" bestFit="1" customWidth="1" style="2" min="8" max="8"/>
+    <col width="14.5703125" bestFit="1" customWidth="1" style="2" min="9" max="9"/>
+    <col width="6.5703125" bestFit="1" customWidth="1" style="2" min="10" max="10"/>
+    <col width="14.5703125" bestFit="1" customWidth="1" style="2" min="11" max="11"/>
+    <col width="6.5703125" bestFit="1" customWidth="1" style="2" min="12" max="12"/>
+    <col width="14.5703125" bestFit="1" customWidth="1" style="2" min="13" max="13"/>
+    <col width="14.5703125" bestFit="1" customWidth="1" style="2" min="15" max="15"/>
+    <col width="11.7109375" bestFit="1" customWidth="1" style="2" min="16" max="16"/>
+    <col width="14.5703125" bestFit="1" customWidth="1" style="2" min="18" max="18"/>
+    <col width="11.7109375" bestFit="1" customWidth="1" style="2" min="19" max="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="1" t="s">
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Specific</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Counting</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>User</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Flow 1</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Error number 1</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Flow 2</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Error number 2</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Flow 3</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Error number 3</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Flow 1</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Error number 1</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Flow 2</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Error number 2</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>Flow 3</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Error number 3</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>1aa80391-9ee3-4bc2-b3d8-a47f10ef6aff</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>37.08028650283813</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>39.06230998039246</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>41.01840925216675</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>36.97933840751648</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>43.10419225692749</v>
+      </c>
+      <c r="K3" t="n">
+        <v>2</v>
+      </c>
+      <c r="L3" t="n">
+        <v>43.13020539283752</v>
+      </c>
+      <c r="M3" t="n">
         <v>1</v>
       </c>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>0245937c-84ae-4007-ab3a-09af505d8ecc</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>39.10344076156616</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>39.07947945594788</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>41.29680323600769</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>39.20200681686401</v>
+      </c>
+      <c r="I4" t="n">
+        <v>1</v>
+      </c>
+      <c r="J4" t="n">
+        <v>55.21794700622559</v>
+      </c>
+      <c r="K4" t="n">
+        <v>7</v>
+      </c>
+      <c r="L4" t="n">
+        <v>41.03132390975952</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>f39b4222-ca9b-466d-9570-241b5d4e61ec</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>55.27820706367493</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>55.25252747535706</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" t="n">
+        <v>51.27736306190491</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>51.25312304496765</v>
+      </c>
+      <c r="I5" t="n">
+        <v>1</v>
+      </c>
+      <c r="J5" t="n">
+        <v>49.12709021568298</v>
+      </c>
+      <c r="K5" t="n">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="L5" t="n">
+        <v>63.43846225738525</v>
+      </c>
+      <c r="M5" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>979bf1da-65ba-4e9d-96f1-dfd799f1a78a</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>53.37133145332336</v>
+      </c>
+      <c r="C6" t="n">
+        <v>2</v>
+      </c>
+      <c r="D6" t="n">
+        <v>97.83309698104858</v>
+      </c>
+      <c r="E6" t="n">
+        <v>5</v>
+      </c>
+      <c r="F6" t="n">
+        <v>49.2720205783844</v>
+      </c>
+      <c r="G6" t="n">
+        <v>2</v>
+      </c>
+      <c r="H6" t="n">
+        <v>57.39985823631287</v>
+      </c>
+      <c r="I6" t="n">
+        <v>10</v>
+      </c>
+      <c r="J6" t="n">
+        <v>61.41867542266846</v>
+      </c>
+      <c r="K6" t="n">
+        <v>16</v>
+      </c>
+      <c r="L6" t="n">
+        <v>45.32001829147339</v>
+      </c>
+      <c r="M6" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>8b3c0a46-1f63-4d19-a248-40222dad6f81</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>43.03067898750305</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>53.26749730110168</v>
+      </c>
+      <c r="E7" t="n">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="F7" t="n">
+        <v>44.98966670036316</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>55.25388097763062</v>
+      </c>
+      <c r="I7" t="n">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="J7" t="n">
+        <v>55.38085436820984</v>
+      </c>
+      <c r="K7" t="n">
+        <v>7</v>
+      </c>
+      <c r="L7" t="n">
+        <v>45.32103157043457</v>
+      </c>
+      <c r="M7" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>eafdc5a2-6fdb-46d2-a807-6c86e55fbb69</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>49.38986468315125</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" t="n">
+        <v>49.30785417556763</v>
+      </c>
+      <c r="E8" t="n">
+        <v>1</v>
+      </c>
+      <c r="F8" t="n">
+        <v>41.17647409439087</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>45.33595681190491</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>47.14960789680481</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" t="n">
+        <v>45.24827742576599</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>3757e6a1-7aef-4dc3-b46c-f0aae5a22e72</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>51.43950128555298</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" t="n">
+        <v>49.32256770133972</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>47.00203704833984</v>
+      </c>
+      <c r="G9" t="n">
+        <v>1</v>
+      </c>
+      <c r="H9" t="n">
+        <v>43.30062890052795</v>
+      </c>
+      <c r="I9" t="n">
+        <v>1</v>
+      </c>
+      <c r="J9" t="n">
+        <v>43.15108680725098</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" t="n">
+        <v>83.71430397033691</v>
+      </c>
+      <c r="M9" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>e2b49249-4d81-43eb-bbb0-67c2bdcc5c9e</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>61.5076789855957</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" t="n">
+        <v>51.17540836334229</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" t="n">
+        <v>43.18260979652405</v>
+      </c>
+      <c r="G10" t="n">
+        <v>1</v>
+      </c>
+      <c r="H10" t="n">
+        <v>47.42498016357422</v>
+      </c>
+      <c r="I10" t="n">
+        <v>4</v>
+      </c>
+      <c r="J10" t="n">
+        <v>69.55706644058228</v>
+      </c>
+      <c r="K10" t="n">
+        <v>10</v>
+      </c>
+      <c r="L10" t="n">
+        <v>53.22811818122864</v>
+      </c>
+      <c r="M10" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>5e56d333-a8c3-4a00-9e2b-589fdc305303</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>65.52746415138245</v>
+      </c>
+      <c r="C11" t="n">
+        <v>13</v>
+      </c>
+      <c r="D11" t="n">
+        <v>49.2728443145752</v>
+      </c>
+      <c r="E11" t="n">
+        <v>4</v>
+      </c>
+      <c r="F11" t="n">
+        <v>47.25991916656494</v>
+      </c>
+      <c r="G11" t="n">
+        <v>2</v>
+      </c>
+      <c r="H11" t="n">
+        <v>59.40259909629822</v>
+      </c>
+      <c r="I11" t="n">
+        <v>8</v>
+      </c>
+      <c r="J11" t="n">
+        <v>49.17812132835388</v>
+      </c>
+      <c r="K11" t="n">
         <v>6</v>
       </c>
-      <c r="F2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J2" t="s">
-        <v>5</v>
-      </c>
-      <c r="K2" t="s">
-        <v>6</v>
-      </c>
-      <c r="L2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M2" t="s">
-        <v>8</v>
+      <c r="L11" t="n">
+        <v>49.16652345657349</v>
+      </c>
+      <c r="M11" t="n">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>